<commit_message>
- Problema e solução: Smarter Phones LTDA
</commit_message>
<xml_diff>
--- a/3. solucao - smarter phones ltda.xlsx
+++ b/3. solucao - smarter phones ltda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.lopes\Documents\mateusbtlopes\simplex-lp-solver-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891FDB3A-A861-4743-B14A-DEC436AA4C1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDAE89B-9BC9-4AFF-96BC-A5D96EF7DD74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -331,7 +331,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,12 +361,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -573,14 +567,11 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -611,17 +602,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -641,10 +632,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -962,50 +959,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1025,30 +1022,30 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <v>0</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="16">
         <v>568.75</v>
       </c>
     </row>
@@ -1058,70 +1055,70 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="17">
         <v>0</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="17">
         <v>3.75</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="17">
         <v>0</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="17">
         <v>2.5</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="18">
         <v>0</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="18">
         <v>0</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="13" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1131,62 +1128,62 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="17">
         <v>25</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="18">
         <v>20</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1213,17 +1210,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1233,113 +1230,113 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="20" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="15">
         <v>3.75</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="15">
         <v>0</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="15">
         <v>85</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="15">
         <v>3.0000000000000004</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="15">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="15">
         <v>2.5</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="15">
         <v>0</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="15">
         <v>100</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="15">
         <v>1.5000000000000002</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="15">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>0</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>1.25</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <v>120</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <v>1E+30</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <v>1.25</v>
       </c>
     </row>
@@ -1349,90 +1346,90 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="19" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="20" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="15">
         <v>25</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="15">
         <v>18.75</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="15">
         <v>25</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="15">
         <v>15</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="15">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="13">
         <v>20</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <v>5</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="13">
         <v>20</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="13">
         <v>11.249999999999998</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="13">
         <v>7.5</v>
       </c>
     </row>
@@ -1462,159 +1459,159 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
-      <c r="C6" s="20" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="20" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>568.75</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="F11" s="20" t="s">
+      <c r="D11" s="19"/>
+      <c r="F11" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="20" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="17">
         <v>3.75</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
         <v>3.75</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="17">
         <v>568.75</v>
       </c>
-      <c r="I13" s="16" t="e">
+      <c r="I13" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J13" s="16" t="e">
+      <c r="J13" s="15" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="17">
         <v>2.5</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="17">
         <v>2.5</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="17">
         <v>568.75</v>
       </c>
-      <c r="I14" s="16" t="e">
+      <c r="I14" s="15" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J14" s="16" t="e">
+      <c r="J14" s="15" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="18">
         <v>0</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="18">
         <v>0</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="18">
         <v>568.75</v>
       </c>
-      <c r="I15" s="14" t="e">
+      <c r="I15" s="13" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J15" s="14" t="e">
+      <c r="J15" s="13" t="e">
         <v>#N/A</v>
       </c>
     </row>
@@ -1627,7 +1624,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1637,135 +1636,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="23"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="21">
         <v>85000</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <v>100000</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="24">
         <v>120000</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>3.75</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>2.5</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="29">
         <f>SUMPRODUCT(C3:E3,C4:E4)</f>
         <v>568750</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="28">
         <v>4</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="28">
         <v>4</v>
       </c>
       <c r="E9" s="1">
         <v>5</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <f>SUMPRODUCT($C$4:$E$4,C9:E9)</f>
         <v>25</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="28">
         <v>2</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="28">
         <v>5</v>
       </c>
       <c r="E10" s="1">
         <v>5</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <f>SUMPRODUCT($C$4:$E$4,C10:E10)</f>
         <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>20</v>
       </c>
     </row>

</xml_diff>